<commit_message>
added a featuer to plot and manually find parameters to better estimate initial guesses
</commit_message>
<xml_diff>
--- a/case2_Glu-Fru/_fructose.xlsx
+++ b/case2_Glu-Fru/_fructose.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\28820169\Downloads\BO Papers\Regression_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\28820169\Downloads\BO_Papers\MEng_Code\case2_Glu-Fru\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7B8FAF-2117-4990-86A9-13F87A005565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1719A4EA-BDA4-4216-BE87-CA495D59614C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="glucose" sheetId="1" r:id="rId1"/>
@@ -210,8 +210,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -358,7 +359,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -371,6 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,10 +703,10 @@
       <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>26</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -766,7 +767,7 @@
         <f>C2*60</f>
         <v>0</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="12">
         <v>0</v>
       </c>
       <c r="F2" s="1">
@@ -779,14 +780,14 @@
       <c r="H2" s="1">
         <v>15</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>70</v>
       </c>
       <c r="J2" s="1">
         <f>H2/I2</f>
         <v>0.21428571428571427</v>
       </c>
-      <c r="K2" s="15">
+      <c r="K2" s="14">
         <f>427.98*(0.001)</f>
         <v>0.42798000000000003</v>
       </c>
@@ -814,7 +815,7 @@
       <c r="S2" s="1">
         <v>0</v>
       </c>
-      <c r="T2" s="5">
+      <c r="T2" s="4">
         <v>0.3</v>
       </c>
     </row>
@@ -833,13 +834,14 @@
         <f t="shared" ref="D3:D27" si="1">C3*60</f>
         <v>48</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="13">
         <v>0</v>
       </c>
       <c r="F3" s="1">
         <f>E3*(1/1000)</f>
         <v>0</v>
       </c>
+      <c r="G3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -856,13 +858,14 @@
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="13">
         <v>0</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" ref="F4:F27" si="2">E4*(1/1000)</f>
         <v>0</v>
       </c>
+      <c r="G4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -879,13 +882,14 @@
         <f t="shared" si="1"/>
         <v>144.00000000000003</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="13">
         <v>0</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="G5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -902,13 +906,14 @@
         <f t="shared" si="1"/>
         <v>192</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="13">
         <v>0</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
@@ -925,13 +930,14 @@
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E7" s="13">
         <v>0</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="G7" s="15"/>
     </row>
     <row r="8" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -948,14 +954,14 @@
         <f t="shared" si="1"/>
         <v>288.00000000000006</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <v>4.266</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <f t="shared" si="2"/>
         <v>4.2659999999999998E-3</v>
       </c>
-      <c r="G8" s="3"/>
+      <c r="G8" s="15"/>
       <c r="H8" s="1" t="s">
         <v>48</v>
       </c>
@@ -979,14 +985,14 @@
         <f t="shared" si="1"/>
         <v>336.00000000000006</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="13">
         <v>33.479999999999997</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <f t="shared" si="2"/>
         <v>3.3479999999999996E-2</v>
       </c>
-      <c r="G9" s="3"/>
+      <c r="G9" s="15"/>
     </row>
     <row r="10" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
@@ -1003,14 +1009,14 @@
         <f t="shared" si="1"/>
         <v>384</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="13">
         <v>141.291</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="5">
         <f t="shared" si="2"/>
         <v>0.141291</v>
       </c>
-      <c r="G10" s="3"/>
+      <c r="G10" s="15"/>
     </row>
     <row r="11" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -1027,14 +1033,14 @@
         <f t="shared" si="1"/>
         <v>432</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="13">
         <v>168.21539999999999</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="5">
         <f t="shared" si="2"/>
         <v>0.16821539999999999</v>
       </c>
-      <c r="G11" s="3"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
@@ -1051,14 +1057,14 @@
         <f t="shared" si="1"/>
         <v>480</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="13">
         <v>208.72080000000003</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="5">
         <f t="shared" si="2"/>
         <v>0.20872080000000004</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="15"/>
     </row>
     <row r="13" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -1075,14 +1081,14 @@
         <f t="shared" si="1"/>
         <v>528</v>
       </c>
-      <c r="E13" s="14">
+      <c r="E13" s="13">
         <v>141.7824</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="5">
         <f t="shared" si="2"/>
         <v>0.1417824</v>
       </c>
-      <c r="G13" s="3"/>
+      <c r="G13" s="15"/>
     </row>
     <row r="14" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -1099,14 +1105,14 @@
         <f t="shared" si="1"/>
         <v>576.00000000000011</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="13">
         <v>110.42999999999999</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F14" s="5">
         <f t="shared" si="2"/>
         <v>0.11043</v>
       </c>
-      <c r="G14" s="3"/>
+      <c r="G14" s="15"/>
     </row>
     <row r="15" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
@@ -1123,14 +1129,14 @@
         <f t="shared" si="1"/>
         <v>624</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="13">
         <v>70.01100000000001</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="5">
         <f t="shared" si="2"/>
         <v>7.0011000000000018E-2</v>
       </c>
-      <c r="G15" s="3"/>
+      <c r="G15" s="15"/>
     </row>
     <row r="16" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
@@ -1147,14 +1153,14 @@
         <f t="shared" si="1"/>
         <v>672.00000000000011</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="13">
         <v>42.3414</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="5">
         <f t="shared" si="2"/>
         <v>4.2341400000000001E-2</v>
       </c>
-      <c r="G16" s="3"/>
+      <c r="G16" s="15"/>
     </row>
     <row r="17" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -1171,14 +1177,14 @@
         <f t="shared" si="1"/>
         <v>720</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="13">
         <v>20.314800000000002</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="5">
         <f t="shared" si="2"/>
         <v>2.0314800000000001E-2</v>
       </c>
-      <c r="G17" s="3"/>
+      <c r="G17" s="15"/>
     </row>
     <row r="18" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -1195,14 +1201,14 @@
         <f t="shared" si="1"/>
         <v>768</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="13">
         <v>6.5717999999999996</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="5">
         <f t="shared" si="2"/>
         <v>6.5718E-3</v>
       </c>
-      <c r="G18" s="3"/>
+      <c r="G18" s="15"/>
     </row>
     <row r="19" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -1219,14 +1225,14 @@
         <f t="shared" si="1"/>
         <v>816.00000000000011</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E19" s="13">
         <v>1.9008</v>
       </c>
-      <c r="F19" s="6">
+      <c r="F19" s="5">
         <f t="shared" si="2"/>
         <v>1.9008E-3</v>
       </c>
-      <c r="G19" s="3"/>
+      <c r="G19" s="15"/>
     </row>
     <row r="20" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
@@ -1243,14 +1249,14 @@
         <f t="shared" si="1"/>
         <v>864</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E20" s="13">
         <v>0.65880000000000005</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="5">
         <f t="shared" si="2"/>
         <v>6.5880000000000008E-4</v>
       </c>
-      <c r="G20" s="3"/>
+      <c r="G20" s="15"/>
     </row>
     <row r="21" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
@@ -1267,14 +1273,14 @@
         <f t="shared" si="1"/>
         <v>912.00000000000011</v>
       </c>
-      <c r="E21" s="14">
-        <v>0</v>
-      </c>
-      <c r="F21" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="3"/>
+      <c r="E21" s="13">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="15"/>
     </row>
     <row r="22" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
@@ -1291,14 +1297,14 @@
         <f t="shared" si="1"/>
         <v>960</v>
       </c>
-      <c r="E22" s="14">
-        <v>0</v>
-      </c>
-      <c r="F22" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="3"/>
+      <c r="E22" s="13">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G22" s="15"/>
     </row>
     <row r="23" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
@@ -1315,14 +1321,14 @@
         <f t="shared" si="1"/>
         <v>1008</v>
       </c>
-      <c r="E23" s="14">
-        <v>0</v>
-      </c>
-      <c r="F23" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="3"/>
+      <c r="E23" s="13">
+        <v>0</v>
+      </c>
+      <c r="F23" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G23" s="15"/>
     </row>
     <row r="24" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
@@ -1339,14 +1345,14 @@
         <f t="shared" si="1"/>
         <v>1056</v>
       </c>
-      <c r="E24" s="14">
-        <v>0</v>
-      </c>
-      <c r="F24" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="3"/>
+      <c r="E24" s="13">
+        <v>0</v>
+      </c>
+      <c r="F24" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="15"/>
     </row>
     <row r="25" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
@@ -1363,14 +1369,14 @@
         <f t="shared" si="1"/>
         <v>1104.0000000000002</v>
       </c>
-      <c r="E25" s="14">
-        <v>0</v>
-      </c>
-      <c r="F25" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="3"/>
+      <c r="E25" s="13">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="15"/>
     </row>
     <row r="26" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -1387,184 +1393,208 @@
         <f t="shared" si="1"/>
         <v>1152.0000000000002</v>
       </c>
-      <c r="E26" s="14">
-        <v>0</v>
-      </c>
-      <c r="F26" s="6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="3"/>
+      <c r="E26" s="13">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="15"/>
     </row>
     <row r="27" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="6">
         <v>25</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <f t="shared" si="1"/>
         <v>1200</v>
       </c>
-      <c r="E27" s="14">
-        <v>0</v>
-      </c>
-      <c r="F27" s="8">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="3"/>
+      <c r="E27" s="13">
+        <v>0</v>
+      </c>
+      <c r="F27" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="15"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="10"/>
-      <c r="F28" s="9"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="15"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E29" s="11"/>
+      <c r="E29" s="10"/>
+      <c r="G29" s="15"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E30" s="11"/>
+      <c r="E30" s="10"/>
+      <c r="G30" s="15"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E31" s="11"/>
+      <c r="E31" s="10"/>
+      <c r="G31" s="15"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E32" s="11"/>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E33" s="11"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E34" s="11"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E35" s="11"/>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E36" s="11"/>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E37" s="11"/>
-    </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E38" s="11"/>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E39" s="11"/>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E40" s="11"/>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E41" s="11"/>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E42" s="11"/>
-    </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E43" s="11"/>
-    </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E44" s="11"/>
-    </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E45" s="11"/>
-    </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E46" s="11"/>
-    </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E47" s="11"/>
-    </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E48" s="11"/>
-    </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E49" s="11"/>
-    </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E50" s="11"/>
-    </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E51" s="12"/>
-    </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E52" s="12"/>
-    </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E53" s="12"/>
-    </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E54" s="12"/>
-    </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E55" s="12"/>
-    </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E56" s="12"/>
-    </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E57" s="12"/>
-    </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E58" s="12"/>
-    </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E59" s="12"/>
-    </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E60" s="12"/>
-    </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E61" s="12"/>
-    </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E62" s="12"/>
-    </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E63" s="12"/>
-    </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E64" s="12"/>
+      <c r="E32" s="10"/>
+      <c r="G32" s="15"/>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E33" s="10"/>
+      <c r="G33" s="15"/>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E34" s="10"/>
+      <c r="G34" s="15"/>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E35" s="10"/>
+      <c r="G35" s="15"/>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E36" s="10"/>
+      <c r="G36" s="15"/>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E37" s="10"/>
+      <c r="G37" s="15"/>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E38" s="10"/>
+      <c r="G38" s="15"/>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E39" s="10"/>
+      <c r="G39" s="15"/>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E40" s="10"/>
+      <c r="G40" s="15"/>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E41" s="10"/>
+      <c r="G41" s="15"/>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E42" s="10"/>
+      <c r="G42" s="15"/>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E43" s="10"/>
+      <c r="G43" s="15"/>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E44" s="10"/>
+      <c r="G44" s="15"/>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E45" s="10"/>
+      <c r="G45" s="15"/>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E46" s="10"/>
+      <c r="G46" s="15"/>
+    </row>
+    <row r="47" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E47" s="10"/>
+      <c r="G47" s="15"/>
+    </row>
+    <row r="48" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E48" s="10"/>
+      <c r="G48" s="15"/>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E49" s="10"/>
+      <c r="G49" s="15"/>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E50" s="10"/>
+      <c r="G50" s="15"/>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E51" s="11"/>
+      <c r="G51" s="15"/>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E52" s="11"/>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E53" s="11"/>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E54" s="11"/>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E55" s="11"/>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E56" s="11"/>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E57" s="11"/>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E58" s="11"/>
+    </row>
+    <row r="59" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E59" s="11"/>
+    </row>
+    <row r="60" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E60" s="11"/>
+    </row>
+    <row r="61" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E61" s="11"/>
+    </row>
+    <row r="62" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E62" s="11"/>
+    </row>
+    <row r="63" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E63" s="11"/>
+    </row>
+    <row r="64" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E64" s="11"/>
     </row>
     <row r="65" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E65" s="12"/>
+      <c r="E65" s="11"/>
     </row>
     <row r="66" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E66" s="12"/>
+      <c r="E66" s="11"/>
     </row>
     <row r="67" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E67" s="12"/>
+      <c r="E67" s="11"/>
     </row>
     <row r="68" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E68" s="12"/>
+      <c r="E68" s="11"/>
     </row>
     <row r="69" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E69" s="12"/>
+      <c r="E69" s="11"/>
     </row>
     <row r="70" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E70" s="12"/>
+      <c r="E70" s="11"/>
     </row>
     <row r="71" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E71" s="12"/>
+      <c r="E71" s="11"/>
     </row>
     <row r="72" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E72" s="12"/>
+      <c r="E72" s="11"/>
     </row>
     <row r="73" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E73" s="12"/>
+      <c r="E73" s="11"/>
     </row>
     <row r="74" spans="5:5" x14ac:dyDescent="0.3">
-      <c r="E74" s="12"/>
+      <c r="E74" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1574,6 +1604,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010048117A934AEAC441AF47E945F1AED0C0" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7272456f5b53c8ae1c345851aef95d27">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c39f1452-4462-4979-941b-c1317cfd14ce" xmlns:ns3="60199b31-2299-4531-8872-a3eaba744cbd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="16ed4d68a838bfbb08a7468a1792fb8f" ns2:_="" ns3:_="">
     <xsd:import namespace="c39f1452-4462-4979-941b-c1317cfd14ce"/>
@@ -1830,16 +1869,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21AAFDFA-AF70-4552-A086-9BCC58150335}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF42137A-B7F2-4A60-BAD9-4B8683F12BBF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1856,12 +1894,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21AAFDFA-AF70-4552-A086-9BCC58150335}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>